<commit_message>
Fix issues after merging SML into master and regenerated outputs after merge
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/composition-sml-prac-1.xlsx
+++ b/output/SharedMedicinesList/composition-sml-prac-1.xlsx
@@ -497,7 +497,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-02:A practitioner role shall conform to PractitionerRole with Practitioner with Mandatory Identifier {extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-withpractitionerident-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-02:A practitioner role shall conform to PractitionerRole with Practitioner with Mandatory Identifier {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-withpractitionerident-1')}</t>
   </si>
   <si>
     <t>informationRecipient</t>
@@ -514,7 +514,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-06:A practitioner shall conform to Base Practitioner {extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-dh-base-1')}inv-dh-cmp-07:A patient shall conform to Base Patient {extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-dh-base-1')}inv-dh-cmp-08:A related person shall conform to Base RelatedPerson {extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}inv-dh-cmp-09:A practitioner role shall conform to Base PractitionerRole {extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-dh-base-1')}inv-dh-cmp-10:An organisation shall conform to Base Organization {extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/organization-dh-base-1')}inv-dh-cmp-11:Information recipient shall not be a device {extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().where($this is Device).exists().not()}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-06:A practitioner shall conform to Base Practitioner {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-dh-base-1')}inv-dh-cmp-07:A patient shall conform to Base Patient {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-dh-base-1')}inv-dh-cmp-08:A related person shall conform to Base RelatedPerson {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}inv-dh-cmp-09:A practitioner role shall conform to Base PractitionerRole {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-dh-base-1')}inv-dh-cmp-10:An organisation shall conform to Base Organization {resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/organization-dh-base-1')}inv-dh-cmp-11:Information recipient shall not be a device {resolve().where($this is Device).exists().not()}</t>
   </si>
   <si>
     <t>Composition.modifierExtension</t>
@@ -1347,7 +1347,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-03:The section shall at least have one entry or an empty reason, but not both {section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '48765-2').entry.exists() xor section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '48765-2').emptyReason.exists()}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-03:The section shall at least have one entry or an empty reason, but not both {entry.exists() xor emptyReason.exists()}</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
@@ -1381,7 +1381,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-04:If present, the assertion of no relevant finding entry shall assert no known current medications {section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '10160-0').exists() implies (section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '10160-0').entry.resolve().where($this is List).exists() xor section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '10160-0').entry.resolve().where($this is Observation ).exists())}inv-dh-cmp-05:The section shall at least have one entry or an empty reason, but not both {section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '10160-0').entry.exists() xor section.where($this.code.coding.system='http://loinc.org' and $this.code.coding.code = '10160-0').emptyReason.exists()}</t>
+cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-04:If present, the assertion of no relevant finding entry shall assert no known current medications {entry.resolve().where($this is Observation ).exists() implies entry.resolve().where($this is value and value.coding.code = '1234391000168107').exists()}inv-dh-cmp-05:The section shall at least have one entry or an empty reason, but not both {entry.exists() xor emptyReason.exists()}</t>
   </si>
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;

</xml_diff>

<commit_message>
Regenerated SML IG outputs
Multiple updates across the SML IG from peer review feedback.
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/composition-sml-prac-1.xlsx
+++ b/output/SharedMedicinesList/composition-sml-prac-1.xlsx
@@ -1002,7 +1002,7 @@
     <t>legalAttester</t>
   </si>
   <si>
-    <t>Legal attester</t>
+    <t>Legal Attester</t>
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
@@ -1453,7 +1453,7 @@
     <t>medications</t>
   </si>
   <si>
-    <t>Medicines list</t>
+    <t>Medicines List</t>
   </si>
   <si>
     <t>Information about medicines. This may include self-prescribed, clinician prescribed and nonprescription medicines, as well as all regular, intermittent and as required medicines pertinent to a patient. Information may also include changes to the therapy, including dose changes, new medicines and ceased medicines.</t>

</xml_diff>

<commit_message>
Regenerate SML IG outputs
Added 4 SML examples, as a variety of Composition, List and Bundle instances.
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/composition-sml-prac-1.xlsx
+++ b/output/SharedMedicinesList/composition-sml-prac-1.xlsx
@@ -1463,7 +1463,7 @@
 cmp-1:A section must at least one of text, entries, or sub-sections {text.exists() or entry.exists() or section.exists()}cmp-2:A section can only have an emptyReason if it is empty {emptyReason.empty() or entry.empty()}inv-dh-cmp-15:The section shall at least have one entry or an empty reason, but not both {entry.exists() xor emptyReason.exists()}inv-dh-cmp-19:A Ceased Medicines section shall not have an assertion of no relevant finding entry {code.coding.where(code='101.32027').exists() implies entry.reference.resolve().where($this is Observation).exists().not()}inv-dh-cmp-16:If present, the assertion of no relevant finding entry shall assert no known current medications {entry.resolve().where($this is Observation ).exists() implies entry.resolve().where($this is value and value.coding.code = '1234391000168107').exists()}inv-dh-cmp-17:If present, a list shall have the same code as the section {entry.resolve().where($this is List).exists() implies ((entry.resolve().code.coding.code) = code.coding.code)}</t>
   </si>
   <si>
-    <t>https://healthterminologies.gov.au/fhir/ValueSet/history-of-medication-use-type-1</t>
+    <t>https://healthterminologies.gov.au/fhir/ValueSet/history-of-medication-use-list-type-1</t>
   </si>
   <si>
     <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/list-sml-pracchanges-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/observation-norelevantfinding-1)
@@ -1652,7 +1652,7 @@
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="95.21875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="75.7109375" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="78.9921875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="40.03515625" customWidth="true" bestFit="true"/>

</xml_diff>

<commit_message>
Build SML with improvements to invariants in Composition and List In Shared Medicines List Authored by Practitioner merge inv-dh-cmp-06 into inv-dh-cmp-01 and fix the xpath in the invariant In List of Medicine Items with Change Information Authored by Practitioner merge inv-dh-lst-05 into inv-dh-lst-03 and fix the xpath in the invariant
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/composition-sml-prac-1.xlsx
+++ b/output/SharedMedicinesList/composition-sml-prac-1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3840" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3840" uniqueCount="462">
   <si>
     <t>Path</t>
   </si>
@@ -153,7 +153,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-cmp-01:The author role shall at least have a reference or an identifier with at least a system and a value {extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').valueReference.reference.exists() or extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').valueReference.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-18:If present, an information recipient shall at least have a reference, an identifier or a display {informationRecipient.exists() implies informationRecipient.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-cmp-02:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-03:The author shall at least have a reference or an identifier with at least a system and a value {author.reference.exists() or author.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-04:The custodian shall at least have a reference or an identifier with at least a system and a value {custodian.reference.exists() or custodian.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource {contained.where(('#'+id in %resource.descendants().reference).not()).empty()}inv-dh-cmp-01:The author role shall at least have a reference to a practitioner role that conforms to PractitionerRole with Practitioner with Mandatory Identifier or an identifier with at least a system and a value {extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').valueReference.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-withpractitionerident-1') or extension('http://hl7.org.au/fhir/StructureDefinition/composition-author-role').valueReference.identifier.where(system.count() + value.count() &gt;1).exists()}inv-dh-cmp-18:If present, an information recipient shall at least have a reference, an identifier or a display {informationRecipient.exists() implies informationRecipient.all($this.reference.exists() or $this.identifier.exists() or $this.display.exists())}inv-dh-cmp-02:The subject shall at least have a reference or an identifier with at least a system and a value {subject.reference.exists() or subject.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-03:The author shall at least have a reference or an identifier with at least a system and a value {author.reference.exists() or author.identifier.where(system.count() + value.count() &gt; 1).exists()}inv-dh-cmp-04:The custodian shall at least have a reference or an identifier with at least a system and a value {custodian.reference.exists() or custodian.identifier.where(system.count() + value.count() &gt; 1).exists()}</t>
   </si>
   <si>
     <t>Document[classCode="DOC" and moodCode="EVN" and isNormalAct()]</t>
@@ -497,7 +497,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-06:A practitioner role shall conform to PractitionerRole with Practitioner with Mandatory Identifier {valueReference.reference.resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-withpractitionerident-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>informationRecipient</t>
@@ -910,10 +910,6 @@
   </si>
   <si>
     <t>A related person that attested this composition.</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
   </si>
   <si>
     <t>Composition.attester.modifierExtension</t>
@@ -5762,7 +5758,7 @@
         <v>152</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>284</v>
+        <v>153</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>39</v>
@@ -5776,11 +5772,11 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" t="s" s="2">
@@ -5805,7 +5801,7 @@
         <v>160</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M39" t="s" s="2">
         <v>74</v>
@@ -5858,7 +5854,7 @@
         <v>39</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>40</v>
@@ -5884,7 +5880,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5910,16 +5906,16 @@
         <v>119</v>
       </c>
       <c r="K40" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="M40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>39</v>
@@ -5947,11 +5943,11 @@
         <v>176</v>
       </c>
       <c r="X40" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="Y40" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="Y40" t="s" s="2">
-        <v>295</v>
-      </c>
       <c r="Z40" t="s" s="2">
         <v>39</v>
       </c>
@@ -5968,7 +5964,7 @@
         <v>39</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>50</v>
@@ -5983,10 +5979,10 @@
         <v>39</v>
       </c>
       <c r="AJ40" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AK40" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>39</v>
@@ -5994,7 +5990,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6020,14 +6016,14 @@
         <v>239</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="L41" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>39</v>
@@ -6076,7 +6072,7 @@
         <v>39</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>40</v>
@@ -6091,10 +6087,10 @@
         <v>39</v>
       </c>
       <c r="AJ41" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AK41" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>39</v>
@@ -6102,7 +6098,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6125,17 +6121,17 @@
         <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="K42" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="L42" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>39</v>
@@ -6184,7 +6180,7 @@
         <v>39</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>40</v>
@@ -6199,13 +6195,13 @@
         <v>39</v>
       </c>
       <c r="AJ42" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AK42" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="AK42" t="s" s="2">
+      <c r="AL42" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AL42" t="s" s="2">
-        <v>311</v>
       </c>
     </row>
     <row r="43">
@@ -6213,7 +6209,7 @@
         <v>268</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C43" t="s" s="2">
         <v>39</v>
@@ -6238,7 +6234,7 @@
         <v>269</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L43" t="s" s="2">
         <v>271</v>
@@ -6308,7 +6304,7 @@
         <v>39</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>276</v>
@@ -6626,7 +6622,7 @@
         <v>152</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>284</v>
+        <v>153</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>39</v>
@@ -6640,11 +6636,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6669,7 +6665,7 @@
         <v>160</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>74</v>
@@ -6722,7 +6718,7 @@
         <v>39</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>40</v>
@@ -6748,7 +6744,7 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6774,23 +6770,23 @@
         <v>119</v>
       </c>
       <c r="K48" t="s" s="2">
+        <v>289</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>290</v>
       </c>
-      <c r="L48" t="s" s="2">
+      <c r="M48" t="s" s="2">
         <v>291</v>
       </c>
-      <c r="M48" t="s" s="2">
+      <c r="N48" t="s" s="2">
         <v>292</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>293</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P48" s="2"/>
       <c r="Q48" t="s" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="R48" t="s" s="2">
         <v>39</v>
@@ -6811,11 +6807,11 @@
         <v>176</v>
       </c>
       <c r="X48" t="s" s="2">
+        <v>293</v>
+      </c>
+      <c r="Y48" t="s" s="2">
         <v>294</v>
       </c>
-      <c r="Y48" t="s" s="2">
-        <v>295</v>
-      </c>
       <c r="Z48" t="s" s="2">
         <v>39</v>
       </c>
@@ -6832,7 +6828,7 @@
         <v>39</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>50</v>
@@ -6847,10 +6843,10 @@
         <v>39</v>
       </c>
       <c r="AJ48" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="AK48" t="s" s="2">
         <v>296</v>
-      </c>
-      <c r="AK48" t="s" s="2">
-        <v>297</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>39</v>
@@ -6858,7 +6854,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6884,14 +6880,14 @@
         <v>239</v>
       </c>
       <c r="K49" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="L49" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="L49" t="s" s="2">
-        <v>300</v>
       </c>
       <c r="M49" s="2"/>
       <c r="N49" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>39</v>
@@ -6940,7 +6936,7 @@
         <v>39</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>40</v>
@@ -6955,10 +6951,10 @@
         <v>39</v>
       </c>
       <c r="AJ49" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AK49" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="AK49" t="s" s="2">
-        <v>303</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>39</v>
@@ -6966,7 +6962,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -6992,14 +6988,14 @@
         <v>248</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="L50" t="s" s="2">
         <v>306</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>307</v>
       </c>
       <c r="M50" s="2"/>
       <c r="N50" t="s" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>39</v>
@@ -7048,7 +7044,7 @@
         <v>39</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>40</v>
@@ -7063,18 +7059,18 @@
         <v>39</v>
       </c>
       <c r="AJ50" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="AK50" t="s" s="2">
         <v>309</v>
       </c>
-      <c r="AK50" t="s" s="2">
+      <c r="AL50" t="s" s="2">
         <v>310</v>
-      </c>
-      <c r="AL50" t="s" s="2">
-        <v>311</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7097,19 +7093,19 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="K51" t="s" s="2">
         <v>317</v>
       </c>
-      <c r="K51" t="s" s="2">
+      <c r="L51" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="L51" t="s" s="2">
+      <c r="M51" t="s" s="2">
         <v>319</v>
       </c>
-      <c r="M51" t="s" s="2">
+      <c r="N51" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>321</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>39</v>
@@ -7158,7 +7154,7 @@
         <v>39</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>40</v>
@@ -7173,10 +7169,10 @@
         <v>39</v>
       </c>
       <c r="AJ51" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="AK51" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="AK51" t="s" s="2">
-        <v>323</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>39</v>
@@ -7184,7 +7180,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7210,13 +7206,13 @@
         <v>269</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="L52" t="s" s="2">
         <v>325</v>
       </c>
-      <c r="L52" t="s" s="2">
+      <c r="M52" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>327</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7266,7 +7262,7 @@
         <v>39</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>40</v>
@@ -7278,13 +7274,13 @@
         <v>39</v>
       </c>
       <c r="AI52" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
         <v>328</v>
       </c>
-      <c r="AJ52" t="s" s="2">
+      <c r="AK52" t="s" s="2">
         <v>329</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>39</v>
@@ -7292,7 +7288,7 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7398,7 +7394,7 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7506,11 +7502,11 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" t="s" s="2">
@@ -7535,7 +7531,7 @@
         <v>160</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M55" t="s" s="2">
         <v>74</v>
@@ -7588,7 +7584,7 @@
         <v>39</v>
       </c>
       <c r="AE55" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF55" t="s" s="2">
         <v>40</v>
@@ -7614,7 +7610,7 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7640,13 +7636,13 @@
         <v>119</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="L56" t="s" s="2">
         <v>335</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="M56" t="s" s="2">
         <v>336</v>
-      </c>
-      <c r="M56" t="s" s="2">
-        <v>337</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" t="s" s="2">
@@ -7675,46 +7671,46 @@
         <v>176</v>
       </c>
       <c r="X56" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="Y56" t="s" s="2">
         <v>338</v>
       </c>
-      <c r="Y56" t="s" s="2">
+      <c r="Z56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE56" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="AF56" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG56" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI56" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ56" t="s" s="2">
         <v>339</v>
       </c>
-      <c r="Z56" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA56" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB56" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC56" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD56" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE56" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="AF56" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG56" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH56" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI56" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ56" t="s" s="2">
+      <c r="AK56" t="s" s="2">
         <v>340</v>
-      </c>
-      <c r="AK56" t="s" s="2">
-        <v>341</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>39</v>
@@ -7722,7 +7718,7 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7745,13 +7741,13 @@
         <v>51</v>
       </c>
       <c r="J57" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="K57" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="K57" t="s" s="2">
+      <c r="L57" t="s" s="2">
         <v>344</v>
-      </c>
-      <c r="L57" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -7802,7 +7798,7 @@
         <v>39</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>50</v>
@@ -7817,10 +7813,10 @@
         <v>39</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="AK57" t="s" s="2">
         <v>346</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>347</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>39</v>
@@ -7828,7 +7824,7 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7854,16 +7850,16 @@
         <v>269</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>349</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="M58" t="s" s="2">
         <v>350</v>
       </c>
-      <c r="M58" t="s" s="2">
+      <c r="N58" t="s" s="2">
         <v>351</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>352</v>
       </c>
       <c r="O58" t="s" s="2">
         <v>39</v>
@@ -7912,7 +7908,7 @@
         <v>39</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>40</v>
@@ -7924,13 +7920,13 @@
         <v>39</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AJ58" t="s" s="2">
+        <v>352</v>
+      </c>
+      <c r="AK58" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="AK58" t="s" s="2">
-        <v>354</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>39</v>
@@ -7938,7 +7934,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -8044,7 +8040,7 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
@@ -8152,11 +8148,11 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" t="s" s="2">
@@ -8181,7 +8177,7 @@
         <v>160</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M61" t="s" s="2">
         <v>74</v>
@@ -8234,7 +8230,7 @@
         <v>39</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>40</v>
@@ -8260,7 +8256,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8286,13 +8282,13 @@
         <v>182</v>
       </c>
       <c r="K62" t="s" s="2">
+        <v>358</v>
+      </c>
+      <c r="L62" t="s" s="2">
         <v>359</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>360</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8321,11 +8317,11 @@
         <v>109</v>
       </c>
       <c r="X62" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="Y62" t="s" s="2">
         <v>362</v>
       </c>
-      <c r="Y62" t="s" s="2">
-        <v>363</v>
-      </c>
       <c r="Z62" t="s" s="2">
         <v>39</v>
       </c>
@@ -8342,7 +8338,7 @@
         <v>39</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>40</v>
@@ -8368,7 +8364,7 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" t="s" s="2">
@@ -8391,13 +8387,13 @@
         <v>51</v>
       </c>
       <c r="J63" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="K63" t="s" s="2">
         <v>365</v>
       </c>
-      <c r="K63" t="s" s="2">
+      <c r="L63" t="s" s="2">
         <v>366</v>
-      </c>
-      <c r="L63" t="s" s="2">
-        <v>367</v>
       </c>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -8448,7 +8444,7 @@
         <v>39</v>
       </c>
       <c r="AE63" t="s" s="2">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AF63" t="s" s="2">
         <v>40</v>
@@ -8474,7 +8470,7 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" t="s" s="2">
@@ -8497,13 +8493,13 @@
         <v>51</v>
       </c>
       <c r="J64" t="s" s="2">
+        <v>368</v>
+      </c>
+      <c r="K64" t="s" s="2">
         <v>369</v>
       </c>
-      <c r="K64" t="s" s="2">
+      <c r="L64" t="s" s="2">
         <v>370</v>
-      </c>
-      <c r="L64" t="s" s="2">
-        <v>371</v>
       </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
@@ -8554,7 +8550,7 @@
         <v>39</v>
       </c>
       <c r="AE64" t="s" s="2">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AF64" t="s" s="2">
         <v>40</v>
@@ -8569,7 +8565,7 @@
         <v>39</v>
       </c>
       <c r="AJ64" t="s" s="2">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AK64" t="s" s="2">
         <v>68</v>
@@ -8580,7 +8576,7 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" t="s" s="2">
@@ -8606,10 +8602,10 @@
         <v>269</v>
       </c>
       <c r="K65" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="L65" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="L65" t="s" s="2">
-        <v>375</v>
       </c>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
@@ -8648,7 +8644,7 @@
         <v>39</v>
       </c>
       <c r="AA65" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AB65" s="2"/>
       <c r="AC65" t="s" s="2">
@@ -8658,7 +8654,7 @@
         <v>77</v>
       </c>
       <c r="AE65" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF65" t="s" s="2">
         <v>40</v>
@@ -8670,13 +8666,13 @@
         <v>39</v>
       </c>
       <c r="AI65" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
         <v>377</v>
       </c>
-      <c r="AJ65" t="s" s="2">
+      <c r="AK65" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="AK65" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="AL65" t="s" s="2">
         <v>39</v>
@@ -8684,7 +8680,7 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" t="s" s="2">
@@ -8790,7 +8786,7 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" t="s" s="2">
@@ -8894,10 +8890,10 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="B68" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="B68" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="C68" t="s" s="2">
         <v>39</v>
@@ -8919,13 +8915,13 @@
         <v>39</v>
       </c>
       <c r="J68" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="K68" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="K68" t="s" s="2">
+      <c r="L68" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="M68" s="2"/>
       <c r="N68" s="2"/>
@@ -8988,7 +8984,7 @@
         <v>152</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>284</v>
+        <v>153</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>39</v>
@@ -9002,11 +8998,11 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" t="s" s="2">
@@ -9031,7 +9027,7 @@
         <v>160</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M69" t="s" s="2">
         <v>74</v>
@@ -9084,7 +9080,7 @@
         <v>39</v>
       </c>
       <c r="AE69" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF69" t="s" s="2">
         <v>40</v>
@@ -9110,11 +9106,11 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" t="s" s="2">
@@ -9136,16 +9132,16 @@
         <v>64</v>
       </c>
       <c r="K70" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="L70" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="L70" t="s" s="2">
+      <c r="M70" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="M70" t="s" s="2">
+      <c r="N70" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="N70" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="O70" t="s" s="2">
         <v>39</v>
@@ -9194,7 +9190,7 @@
         <v>39</v>
       </c>
       <c r="AE70" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AF70" t="s" s="2">
         <v>40</v>
@@ -9220,7 +9216,7 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" t="s" s="2">
@@ -9246,16 +9242,16 @@
         <v>182</v>
       </c>
       <c r="K71" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L71" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="L71" t="s" s="2">
+      <c r="M71" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="M71" t="s" s="2">
+      <c r="N71" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="N71" t="s" s="2">
-        <v>397</v>
       </c>
       <c r="O71" t="s" s="2">
         <v>39</v>
@@ -9283,11 +9279,11 @@
         <v>109</v>
       </c>
       <c r="X71" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="Y71" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="Y71" t="s" s="2">
-        <v>399</v>
-      </c>
       <c r="Z71" t="s" s="2">
         <v>39</v>
       </c>
@@ -9304,7 +9300,7 @@
         <v>39</v>
       </c>
       <c r="AE71" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AF71" t="s" s="2">
         <v>40</v>
@@ -9330,7 +9326,7 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" t="s" s="2">
@@ -9356,13 +9352,13 @@
         <v>129</v>
       </c>
       <c r="K72" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L72" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="L72" t="s" s="2">
+      <c r="M72" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="M72" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" t="s" s="2">
@@ -9412,7 +9408,7 @@
         <v>39</v>
       </c>
       <c r="AE72" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AF72" t="s" s="2">
         <v>40</v>
@@ -9421,16 +9417,16 @@
         <v>50</v>
       </c>
       <c r="AH72" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AI72" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ72" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="AI72" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ72" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="AK72" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AL72" t="s" s="2">
         <v>39</v>
@@ -9438,7 +9434,7 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" t="s" s="2">
@@ -9464,16 +9460,16 @@
         <v>119</v>
       </c>
       <c r="K73" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L73" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="L73" t="s" s="2">
+      <c r="M73" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="M73" t="s" s="2">
+      <c r="N73" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="N73" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="O73" t="s" s="2">
         <v>39</v>
@@ -9501,43 +9497,43 @@
         <v>176</v>
       </c>
       <c r="X73" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="Y73" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="Y73" t="s" s="2">
+      <c r="Z73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE73" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="AF73" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG73" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI73" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ73" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="Z73" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA73" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB73" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC73" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD73" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE73" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="AF73" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG73" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH73" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI73" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ73" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="AK73" t="s" s="2">
         <v>68</v>
@@ -9548,7 +9544,7 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" t="s" s="2">
@@ -9574,16 +9570,16 @@
         <v>182</v>
       </c>
       <c r="K74" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L74" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="L74" t="s" s="2">
+      <c r="M74" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="M74" t="s" s="2">
+      <c r="N74" t="s" s="2">
         <v>417</v>
-      </c>
-      <c r="N74" t="s" s="2">
-        <v>418</v>
       </c>
       <c r="O74" t="s" s="2">
         <v>39</v>
@@ -9611,43 +9607,43 @@
         <v>188</v>
       </c>
       <c r="X74" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="Y74" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="Y74" t="s" s="2">
+      <c r="Z74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE74" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="AF74" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG74" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI74" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ74" t="s" s="2">
         <v>420</v>
-      </c>
-      <c r="Z74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE74" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="AF74" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG74" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI74" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ74" t="s" s="2">
-        <v>421</v>
       </c>
       <c r="AK74" t="s" s="2">
         <v>68</v>
@@ -9658,7 +9654,7 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" t="s" s="2">
@@ -9681,16 +9677,16 @@
         <v>39</v>
       </c>
       <c r="J75" t="s" s="2">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K75" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="L75" t="s" s="2">
         <v>423</v>
       </c>
-      <c r="L75" t="s" s="2">
+      <c r="M75" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="M75" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" t="s" s="2">
@@ -9740,7 +9736,7 @@
         <v>39</v>
       </c>
       <c r="AE75" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AF75" t="s" s="2">
         <v>40</v>
@@ -9749,16 +9745,16 @@
         <v>41</v>
       </c>
       <c r="AH75" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="AI75" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ75" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="AI75" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ75" t="s" s="2">
+      <c r="AK75" t="s" s="2">
         <v>427</v>
-      </c>
-      <c r="AK75" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>39</v>
@@ -9766,7 +9762,7 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" t="s" s="2">
@@ -9792,16 +9788,16 @@
         <v>182</v>
       </c>
       <c r="K76" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="L76" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="L76" t="s" s="2">
+      <c r="M76" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="M76" t="s" s="2">
+      <c r="N76" t="s" s="2">
         <v>432</v>
-      </c>
-      <c r="N76" t="s" s="2">
-        <v>433</v>
       </c>
       <c r="O76" t="s" s="2">
         <v>39</v>
@@ -9829,43 +9825,43 @@
         <v>188</v>
       </c>
       <c r="X76" t="s" s="2">
+        <v>433</v>
+      </c>
+      <c r="Y76" t="s" s="2">
         <v>434</v>
       </c>
-      <c r="Y76" t="s" s="2">
+      <c r="Z76" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA76" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB76" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC76" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD76" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE76" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="AF76" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG76" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH76" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="AI76" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ76" t="s" s="2">
         <v>435</v>
-      </c>
-      <c r="Z76" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA76" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB76" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC76" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD76" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE76" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="AF76" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG76" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH76" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="AI76" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ76" t="s" s="2">
-        <v>436</v>
       </c>
       <c r="AK76" t="s" s="2">
         <v>68</v>
@@ -9876,7 +9872,7 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" t="s" s="2">
@@ -9902,13 +9898,13 @@
         <v>39</v>
       </c>
       <c r="K77" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="L77" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="L77" t="s" s="2">
+      <c r="M77" t="s" s="2">
         <v>439</v>
-      </c>
-      <c r="M77" t="s" s="2">
-        <v>440</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" t="s" s="2">
@@ -9958,7 +9954,7 @@
         <v>39</v>
       </c>
       <c r="AE77" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AF77" t="s" s="2">
         <v>40</v>
@@ -9967,16 +9963,16 @@
         <v>41</v>
       </c>
       <c r="AH77" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AI77" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ77" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AL77" t="s" s="2">
         <v>39</v>
@@ -9984,10 +9980,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C78" t="s" s="2">
         <v>39</v>
@@ -10012,10 +10008,10 @@
         <v>269</v>
       </c>
       <c r="K78" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="L78" t="s" s="2">
         <v>443</v>
-      </c>
-      <c r="L78" t="s" s="2">
-        <v>444</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -10066,7 +10062,7 @@
         <v>39</v>
       </c>
       <c r="AE78" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF78" t="s" s="2">
         <v>40</v>
@@ -10078,13 +10074,13 @@
         <v>39</v>
       </c>
       <c r="AI78" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AJ78" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="AK78" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="AK78" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="AL78" t="s" s="2">
         <v>39</v>
@@ -10092,7 +10088,7 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" t="s" s="2">
@@ -10198,7 +10194,7 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" t="s" s="2">
@@ -10302,10 +10298,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="B81" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="B81" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="C81" t="s" s="2">
         <v>39</v>
@@ -10327,13 +10323,13 @@
         <v>39</v>
       </c>
       <c r="J81" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="K81" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="K81" t="s" s="2">
+      <c r="L81" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="L81" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -10396,7 +10392,7 @@
         <v>152</v>
       </c>
       <c r="AI81" t="s" s="2">
-        <v>284</v>
+        <v>153</v>
       </c>
       <c r="AJ81" t="s" s="2">
         <v>39</v>
@@ -10410,11 +10406,11 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" t="s" s="2">
@@ -10439,7 +10435,7 @@
         <v>160</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M82" t="s" s="2">
         <v>74</v>
@@ -10492,7 +10488,7 @@
         <v>39</v>
       </c>
       <c r="AE82" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF82" t="s" s="2">
         <v>40</v>
@@ -10518,11 +10514,11 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" t="s" s="2">
@@ -10544,16 +10540,16 @@
         <v>64</v>
       </c>
       <c r="K83" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="L83" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="L83" t="s" s="2">
+      <c r="M83" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="M83" t="s" s="2">
+      <c r="N83" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="N83" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="O83" t="s" s="2">
         <v>39</v>
@@ -10602,7 +10598,7 @@
         <v>39</v>
       </c>
       <c r="AE83" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AF83" t="s" s="2">
         <v>40</v>
@@ -10628,7 +10624,7 @@
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s" s="2">
@@ -10654,23 +10650,23 @@
         <v>182</v>
       </c>
       <c r="K84" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L84" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="L84" t="s" s="2">
+      <c r="M84" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="M84" t="s" s="2">
+      <c r="N84" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="N84" t="s" s="2">
-        <v>397</v>
       </c>
       <c r="O84" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P84" s="2"/>
       <c r="Q84" t="s" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="R84" t="s" s="2">
         <v>39</v>
@@ -10691,11 +10687,11 @@
         <v>109</v>
       </c>
       <c r="X84" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="Y84" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="Y84" t="s" s="2">
-        <v>399</v>
-      </c>
       <c r="Z84" t="s" s="2">
         <v>39</v>
       </c>
@@ -10712,7 +10708,7 @@
         <v>39</v>
       </c>
       <c r="AE84" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AF84" t="s" s="2">
         <v>40</v>
@@ -10738,7 +10734,7 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s" s="2">
@@ -10764,13 +10760,13 @@
         <v>129</v>
       </c>
       <c r="K85" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L85" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="L85" t="s" s="2">
+      <c r="M85" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="M85" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="N85" s="2"/>
       <c r="O85" t="s" s="2">
@@ -10820,7 +10816,7 @@
         <v>39</v>
       </c>
       <c r="AE85" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AF85" t="s" s="2">
         <v>40</v>
@@ -10829,16 +10825,16 @@
         <v>50</v>
       </c>
       <c r="AH85" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AI85" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ85" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="AI85" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ85" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="AK85" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AL85" t="s" s="2">
         <v>39</v>
@@ -10846,7 +10842,7 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s" s="2">
@@ -10872,23 +10868,23 @@
         <v>119</v>
       </c>
       <c r="K86" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L86" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="L86" t="s" s="2">
+      <c r="M86" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="M86" t="s" s="2">
+      <c r="N86" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="N86" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="O86" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P86" s="2"/>
       <c r="Q86" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="R86" t="s" s="2">
         <v>39</v>
@@ -10909,43 +10905,43 @@
         <v>176</v>
       </c>
       <c r="X86" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="Y86" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="Y86" t="s" s="2">
+      <c r="Z86" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA86" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB86" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC86" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD86" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE86" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="AF86" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG86" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH86" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI86" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ86" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="Z86" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA86" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB86" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC86" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD86" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE86" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="AF86" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG86" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH86" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI86" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ86" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="AK86" t="s" s="2">
         <v>68</v>
@@ -10956,7 +10952,7 @@
     </row>
     <row r="87" hidden="true">
       <c r="A87" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s" s="2">
@@ -10982,16 +10978,16 @@
         <v>182</v>
       </c>
       <c r="K87" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L87" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="L87" t="s" s="2">
+      <c r="M87" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="M87" t="s" s="2">
+      <c r="N87" t="s" s="2">
         <v>417</v>
-      </c>
-      <c r="N87" t="s" s="2">
-        <v>418</v>
       </c>
       <c r="O87" t="s" s="2">
         <v>39</v>
@@ -11019,43 +11015,43 @@
         <v>188</v>
       </c>
       <c r="X87" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="Y87" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="Y87" t="s" s="2">
+      <c r="Z87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE87" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="AF87" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG87" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI87" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ87" t="s" s="2">
         <v>420</v>
-      </c>
-      <c r="Z87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE87" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="AF87" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG87" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI87" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ87" t="s" s="2">
-        <v>421</v>
       </c>
       <c r="AK87" t="s" s="2">
         <v>68</v>
@@ -11066,7 +11062,7 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s" s="2">
@@ -11089,16 +11085,16 @@
         <v>39</v>
       </c>
       <c r="J88" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="K88" t="s" s="2">
         <v>448</v>
       </c>
-      <c r="K88" t="s" s="2">
-        <v>449</v>
-      </c>
       <c r="L88" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="M88" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="M88" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="N88" s="2"/>
       <c r="O88" t="s" s="2">
@@ -11148,7 +11144,7 @@
         <v>39</v>
       </c>
       <c r="AE88" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AF88" t="s" s="2">
         <v>40</v>
@@ -11157,16 +11153,16 @@
         <v>41</v>
       </c>
       <c r="AH88" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="AI88" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ88" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="AI88" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ88" t="s" s="2">
+      <c r="AK88" t="s" s="2">
         <v>427</v>
-      </c>
-      <c r="AK88" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="AL88" t="s" s="2">
         <v>39</v>
@@ -11174,7 +11170,7 @@
     </row>
     <row r="89" hidden="true">
       <c r="A89" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s" s="2">
@@ -11280,7 +11276,7 @@
     </row>
     <row r="90" hidden="true">
       <c r="A90" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s" s="2">
@@ -11388,7 +11384,7 @@
     </row>
     <row r="91" hidden="true">
       <c r="A91" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s" s="2">
@@ -11496,7 +11492,7 @@
     </row>
     <row r="92" hidden="true">
       <c r="A92" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s" s="2">
@@ -11604,7 +11600,7 @@
     </row>
     <row r="93" hidden="true">
       <c r="A93" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s" s="2">
@@ -11712,7 +11708,7 @@
     </row>
     <row r="94">
       <c r="A94" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s" s="2">
@@ -11738,16 +11734,16 @@
         <v>182</v>
       </c>
       <c r="K94" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="L94" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="L94" t="s" s="2">
+      <c r="M94" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="M94" t="s" s="2">
+      <c r="N94" t="s" s="2">
         <v>432</v>
-      </c>
-      <c r="N94" t="s" s="2">
-        <v>433</v>
       </c>
       <c r="O94" t="s" s="2">
         <v>39</v>
@@ -11776,7 +11772,7 @@
       </c>
       <c r="X94" s="2"/>
       <c r="Y94" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="Z94" t="s" s="2">
         <v>39</v>
@@ -11794,7 +11790,7 @@
         <v>39</v>
       </c>
       <c r="AE94" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AF94" t="s" s="2">
         <v>40</v>
@@ -11803,13 +11799,13 @@
         <v>50</v>
       </c>
       <c r="AH94" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AI94" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ94" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AK94" t="s" s="2">
         <v>68</v>
@@ -11820,7 +11816,7 @@
     </row>
     <row r="95" hidden="true">
       <c r="A95" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B95" s="2"/>
       <c r="C95" t="s" s="2">
@@ -11846,13 +11842,13 @@
         <v>39</v>
       </c>
       <c r="K95" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="L95" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="L95" t="s" s="2">
+      <c r="M95" t="s" s="2">
         <v>439</v>
-      </c>
-      <c r="M95" t="s" s="2">
-        <v>440</v>
       </c>
       <c r="N95" s="2"/>
       <c r="O95" t="s" s="2">
@@ -11902,7 +11898,7 @@
         <v>39</v>
       </c>
       <c r="AE95" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AF95" t="s" s="2">
         <v>40</v>
@@ -11911,16 +11907,16 @@
         <v>41</v>
       </c>
       <c r="AH95" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AI95" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ95" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AK95" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AL95" t="s" s="2">
         <v>39</v>
@@ -11928,10 +11924,10 @@
     </row>
     <row r="96">
       <c r="A96" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B96" t="s" s="2">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C96" t="s" s="2">
         <v>39</v>
@@ -11956,10 +11952,10 @@
         <v>269</v>
       </c>
       <c r="K96" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="L96" t="s" s="2">
         <v>457</v>
-      </c>
-      <c r="L96" t="s" s="2">
-        <v>458</v>
       </c>
       <c r="M96" s="2"/>
       <c r="N96" s="2"/>
@@ -12010,7 +12006,7 @@
         <v>39</v>
       </c>
       <c r="AE96" t="s" s="2">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AF96" t="s" s="2">
         <v>40</v>
@@ -12022,13 +12018,13 @@
         <v>39</v>
       </c>
       <c r="AI96" t="s" s="2">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="AJ96" t="s" s="2">
+        <v>377</v>
+      </c>
+      <c r="AK96" t="s" s="2">
         <v>378</v>
-      </c>
-      <c r="AK96" t="s" s="2">
-        <v>379</v>
       </c>
       <c r="AL96" t="s" s="2">
         <v>39</v>
@@ -12036,7 +12032,7 @@
     </row>
     <row r="97" hidden="true">
       <c r="A97" t="s" s="2">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B97" s="2"/>
       <c r="C97" t="s" s="2">
@@ -12142,7 +12138,7 @@
     </row>
     <row r="98" hidden="true">
       <c r="A98" t="s" s="2">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" t="s" s="2">
@@ -12246,10 +12242,10 @@
     </row>
     <row r="99" hidden="true">
       <c r="A99" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="B99" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="B99" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="C99" t="s" s="2">
         <v>39</v>
@@ -12271,13 +12267,13 @@
         <v>39</v>
       </c>
       <c r="J99" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="K99" t="s" s="2">
         <v>383</v>
       </c>
-      <c r="K99" t="s" s="2">
+      <c r="L99" t="s" s="2">
         <v>384</v>
-      </c>
-      <c r="L99" t="s" s="2">
-        <v>385</v>
       </c>
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
@@ -12340,7 +12336,7 @@
         <v>152</v>
       </c>
       <c r="AI99" t="s" s="2">
-        <v>284</v>
+        <v>153</v>
       </c>
       <c r="AJ99" t="s" s="2">
         <v>39</v>
@@ -12354,11 +12350,11 @@
     </row>
     <row r="100" hidden="true">
       <c r="A100" t="s" s="2">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B100" s="2"/>
       <c r="C100" t="s" s="2">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" t="s" s="2">
@@ -12383,7 +12379,7 @@
         <v>160</v>
       </c>
       <c r="L100" t="s" s="2">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="M100" t="s" s="2">
         <v>74</v>
@@ -12436,7 +12432,7 @@
         <v>39</v>
       </c>
       <c r="AE100" t="s" s="2">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AF100" t="s" s="2">
         <v>40</v>
@@ -12462,11 +12458,11 @@
     </row>
     <row r="101">
       <c r="A101" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B101" s="2"/>
       <c r="C101" t="s" s="2">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" t="s" s="2">
@@ -12488,16 +12484,16 @@
         <v>64</v>
       </c>
       <c r="K101" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="L101" t="s" s="2">
         <v>389</v>
       </c>
-      <c r="L101" t="s" s="2">
+      <c r="M101" t="s" s="2">
         <v>390</v>
       </c>
-      <c r="M101" t="s" s="2">
+      <c r="N101" t="s" s="2">
         <v>391</v>
-      </c>
-      <c r="N101" t="s" s="2">
-        <v>392</v>
       </c>
       <c r="O101" t="s" s="2">
         <v>39</v>
@@ -12546,7 +12542,7 @@
         <v>39</v>
       </c>
       <c r="AE101" t="s" s="2">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AF101" t="s" s="2">
         <v>40</v>
@@ -12572,7 +12568,7 @@
     </row>
     <row r="102">
       <c r="A102" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B102" s="2"/>
       <c r="C102" t="s" s="2">
@@ -12598,16 +12594,16 @@
         <v>182</v>
       </c>
       <c r="K102" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="L102" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="L102" t="s" s="2">
+      <c r="M102" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="M102" t="s" s="2">
+      <c r="N102" t="s" s="2">
         <v>396</v>
-      </c>
-      <c r="N102" t="s" s="2">
-        <v>397</v>
       </c>
       <c r="O102" t="s" s="2">
         <v>39</v>
@@ -12636,7 +12632,7 @@
       </c>
       <c r="X102" s="2"/>
       <c r="Y102" t="s" s="2">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="Z102" t="s" s="2">
         <v>39</v>
@@ -12654,7 +12650,7 @@
         <v>39</v>
       </c>
       <c r="AE102" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AF102" t="s" s="2">
         <v>40</v>
@@ -12680,7 +12676,7 @@
     </row>
     <row r="103">
       <c r="A103" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B103" s="2"/>
       <c r="C103" t="s" s="2">
@@ -12706,13 +12702,13 @@
         <v>129</v>
       </c>
       <c r="K103" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="L103" t="s" s="2">
         <v>401</v>
       </c>
-      <c r="L103" t="s" s="2">
+      <c r="M103" t="s" s="2">
         <v>402</v>
-      </c>
-      <c r="M103" t="s" s="2">
-        <v>403</v>
       </c>
       <c r="N103" s="2"/>
       <c r="O103" t="s" s="2">
@@ -12762,7 +12758,7 @@
         <v>39</v>
       </c>
       <c r="AE103" t="s" s="2">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AF103" t="s" s="2">
         <v>40</v>
@@ -12771,16 +12767,16 @@
         <v>50</v>
       </c>
       <c r="AH103" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="AI103" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ103" t="s" s="2">
         <v>404</v>
       </c>
-      <c r="AI103" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ103" t="s" s="2">
-        <v>405</v>
-      </c>
       <c r="AK103" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AL103" t="s" s="2">
         <v>39</v>
@@ -12788,7 +12784,7 @@
     </row>
     <row r="104" hidden="true">
       <c r="A104" t="s" s="2">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B104" s="2"/>
       <c r="C104" t="s" s="2">
@@ -12814,23 +12810,23 @@
         <v>119</v>
       </c>
       <c r="K104" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="L104" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="L104" t="s" s="2">
+      <c r="M104" t="s" s="2">
         <v>408</v>
       </c>
-      <c r="M104" t="s" s="2">
+      <c r="N104" t="s" s="2">
         <v>409</v>
-      </c>
-      <c r="N104" t="s" s="2">
-        <v>410</v>
       </c>
       <c r="O104" t="s" s="2">
         <v>39</v>
       </c>
       <c r="P104" s="2"/>
       <c r="Q104" t="s" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="R104" t="s" s="2">
         <v>39</v>
@@ -12851,43 +12847,43 @@
         <v>176</v>
       </c>
       <c r="X104" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="Y104" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="Y104" t="s" s="2">
+      <c r="Z104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE104" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="AF104" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG104" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI104" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ104" t="s" s="2">
         <v>412</v>
-      </c>
-      <c r="Z104" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA104" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB104" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC104" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD104" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE104" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="AF104" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG104" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH104" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI104" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ104" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="AK104" t="s" s="2">
         <v>68</v>
@@ -12898,7 +12894,7 @@
     </row>
     <row r="105" hidden="true">
       <c r="A105" t="s" s="2">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B105" s="2"/>
       <c r="C105" t="s" s="2">
@@ -12924,16 +12920,16 @@
         <v>182</v>
       </c>
       <c r="K105" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="L105" t="s" s="2">
         <v>415</v>
       </c>
-      <c r="L105" t="s" s="2">
+      <c r="M105" t="s" s="2">
         <v>416</v>
       </c>
-      <c r="M105" t="s" s="2">
+      <c r="N105" t="s" s="2">
         <v>417</v>
-      </c>
-      <c r="N105" t="s" s="2">
-        <v>418</v>
       </c>
       <c r="O105" t="s" s="2">
         <v>39</v>
@@ -12961,43 +12957,43 @@
         <v>188</v>
       </c>
       <c r="X105" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="Y105" t="s" s="2">
         <v>419</v>
       </c>
-      <c r="Y105" t="s" s="2">
+      <c r="Z105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE105" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="AF105" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AG105" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI105" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ105" t="s" s="2">
         <v>420</v>
-      </c>
-      <c r="Z105" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA105" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB105" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC105" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD105" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE105" t="s" s="2">
-        <v>414</v>
-      </c>
-      <c r="AF105" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AG105" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH105" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI105" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ105" t="s" s="2">
-        <v>421</v>
       </c>
       <c r="AK105" t="s" s="2">
         <v>68</v>
@@ -13008,7 +13004,7 @@
     </row>
     <row r="106">
       <c r="A106" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" t="s" s="2">
@@ -13031,16 +13027,16 @@
         <v>39</v>
       </c>
       <c r="J106" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="K106" t="s" s="2">
         <v>461</v>
       </c>
-      <c r="K106" t="s" s="2">
-        <v>462</v>
-      </c>
       <c r="L106" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="M106" t="s" s="2">
         <v>424</v>
-      </c>
-      <c r="M106" t="s" s="2">
-        <v>425</v>
       </c>
       <c r="N106" s="2"/>
       <c r="O106" t="s" s="2">
@@ -13090,7 +13086,7 @@
         <v>39</v>
       </c>
       <c r="AE106" t="s" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AF106" t="s" s="2">
         <v>40</v>
@@ -13099,16 +13095,16 @@
         <v>41</v>
       </c>
       <c r="AH106" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="AI106" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ106" t="s" s="2">
         <v>426</v>
       </c>
-      <c r="AI106" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ106" t="s" s="2">
+      <c r="AK106" t="s" s="2">
         <v>427</v>
-      </c>
-      <c r="AK106" t="s" s="2">
-        <v>428</v>
       </c>
       <c r="AL106" t="s" s="2">
         <v>39</v>
@@ -13116,7 +13112,7 @@
     </row>
     <row r="107" hidden="true">
       <c r="A107" t="s" s="2">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B107" s="2"/>
       <c r="C107" t="s" s="2">
@@ -13222,7 +13218,7 @@
     </row>
     <row r="108" hidden="true">
       <c r="A108" t="s" s="2">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B108" s="2"/>
       <c r="C108" t="s" s="2">
@@ -13330,7 +13326,7 @@
     </row>
     <row r="109" hidden="true">
       <c r="A109" t="s" s="2">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B109" s="2"/>
       <c r="C109" t="s" s="2">
@@ -13438,7 +13434,7 @@
     </row>
     <row r="110" hidden="true">
       <c r="A110" t="s" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B110" s="2"/>
       <c r="C110" t="s" s="2">
@@ -13546,7 +13542,7 @@
     </row>
     <row r="111" hidden="true">
       <c r="A111" t="s" s="2">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B111" s="2"/>
       <c r="C111" t="s" s="2">
@@ -13654,7 +13650,7 @@
     </row>
     <row r="112">
       <c r="A112" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B112" s="2"/>
       <c r="C112" t="s" s="2">
@@ -13680,16 +13676,16 @@
         <v>182</v>
       </c>
       <c r="K112" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="L112" t="s" s="2">
         <v>430</v>
       </c>
-      <c r="L112" t="s" s="2">
+      <c r="M112" t="s" s="2">
         <v>431</v>
       </c>
-      <c r="M112" t="s" s="2">
+      <c r="N112" t="s" s="2">
         <v>432</v>
-      </c>
-      <c r="N112" t="s" s="2">
-        <v>433</v>
       </c>
       <c r="O112" t="s" s="2">
         <v>39</v>
@@ -13718,7 +13714,7 @@
       </c>
       <c r="X112" s="2"/>
       <c r="Y112" t="s" s="2">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="Z112" t="s" s="2">
         <v>39</v>
@@ -13736,7 +13732,7 @@
         <v>39</v>
       </c>
       <c r="AE112" t="s" s="2">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AF112" t="s" s="2">
         <v>40</v>
@@ -13745,13 +13741,13 @@
         <v>50</v>
       </c>
       <c r="AH112" t="s" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AI112" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ112" t="s" s="2">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="AK112" t="s" s="2">
         <v>68</v>
@@ -13762,7 +13758,7 @@
     </row>
     <row r="113" hidden="true">
       <c r="A113" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B113" s="2"/>
       <c r="C113" t="s" s="2">
@@ -13788,13 +13784,13 @@
         <v>39</v>
       </c>
       <c r="K113" t="s" s="2">
+        <v>437</v>
+      </c>
+      <c r="L113" t="s" s="2">
         <v>438</v>
       </c>
-      <c r="L113" t="s" s="2">
+      <c r="M113" t="s" s="2">
         <v>439</v>
-      </c>
-      <c r="M113" t="s" s="2">
-        <v>440</v>
       </c>
       <c r="N113" s="2"/>
       <c r="O113" t="s" s="2">
@@ -13844,7 +13840,7 @@
         <v>39</v>
       </c>
       <c r="AE113" t="s" s="2">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="AF113" t="s" s="2">
         <v>40</v>
@@ -13853,16 +13849,16 @@
         <v>41</v>
       </c>
       <c r="AH113" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AI113" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AJ113" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AK113" t="s" s="2">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="AL113" t="s" s="2">
         <v>39</v>

</xml_diff>